<commit_message>
Added agent markedForDeath and ThermalMap now stores numThermals
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hombo\Documents\Github Repositories\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\Code of Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290869F2-18AB-4252-AC46-FA51C823393D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914BD2EA-2039-41C3-A114-8BD75F5201A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -799,7 +799,7 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -1264,7 +1264,7 @@
         <v>93</v>
       </c>
       <c r="C68">
-        <v>200</v>
+        <v>50</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Big change with MasterScriptAdam which now uses Excel SimLaw and MainScriptFunction
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hombo\Documents\Github Repositories\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\Code of Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914BD2EA-2039-41C3-A114-8BD75F5201A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28844363-A925-4025-B7E6-57CC41F53D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="117">
   <si>
     <t>dt</t>
   </si>
@@ -379,6 +379,12 @@
   </si>
   <si>
     <t>simIDNum</t>
+  </si>
+  <si>
+    <t>collisionKillDistance</t>
+  </si>
+  <si>
+    <t>stopWhenDead</t>
   </si>
 </sst>
 </file>
@@ -708,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -755,7 +761,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1200</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -802,31 +808,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>2600</v>
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -834,253 +837,253 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>31</v>
       </c>
-      <c r="C20">
+      <c r="C21">
         <v>9.81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B24" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C25" s="2">
         <v>100000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>36</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>35</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B27" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C28" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>40</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>39</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B30" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
         <v>42</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31">
-        <v>-3</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C32">
-        <v>10</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C33">
-        <v>0.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C34">
-        <v>4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
         <v>52</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>51</v>
       </c>
-      <c r="C35">
+      <c r="C36">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A37" s="1"/>
-      <c r="B37" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" s="1"/>
+      <c r="B38" t="s">
         <v>54</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C38" s="2">
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B39" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
         <v>56</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A40" s="3" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>57</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A42" s="1" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43">
-        <v>1000</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C44">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C45">
         <v>5</v>
@@ -1091,22 +1094,21 @@
         <v>24</v>
       </c>
       <c r="B46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C46">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47">
-        <f>-5/12*PI()</f>
-        <v>-1.3089969389957472</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
@@ -1114,117 +1116,124 @@
         <v>67</v>
       </c>
       <c r="B48" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48">
+        <f>-5/12*PI()</f>
+        <v>-1.3089969389957472</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" t="s">
         <v>68</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <f>5/12*PI()</f>
         <v>1.3089969389957472</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
         <v>70</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>69</v>
       </c>
-      <c r="C49">
+      <c r="C50">
         <f>11/6*PI()</f>
         <v>5.7595865315812871</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B50" t="s">
-        <v>71</v>
-      </c>
-      <c r="C50">
-        <v>-1.8429999999999998E-2</v>
-      </c>
-    </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B51" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C51">
-        <v>0.37819999999999998</v>
+        <v>-1.8429999999999998E-2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52">
+        <v>0.37819999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B53" t="s">
         <v>73</v>
       </c>
-      <c r="C52">
+      <c r="C53">
         <f>-2.3782</f>
         <v>-2.3782000000000001</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A54" s="1" t="s">
+      <c r="A54" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A56" s="1" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B55" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B56" t="s">
-        <v>77</v>
-      </c>
-      <c r="C56" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C57" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>83</v>
-      </c>
       <c r="B58" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C58" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B59" t="s">
-        <v>84</v>
-      </c>
-      <c r="C59" s="4" t="b">
-        <v>1</v>
+        <v>79</v>
+      </c>
+      <c r="C59" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>83</v>
+      </c>
       <c r="B60" t="s">
-        <v>85</v>
-      </c>
-      <c r="C60" t="b">
-        <v>1</v>
+        <v>81</v>
+      </c>
+      <c r="C60" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
-        <v>86</v>
-      </c>
-      <c r="C61" t="b">
-        <v>0</v>
+        <v>84</v>
+      </c>
+      <c r="C61" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B62" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C62" t="b">
         <v>1</v>
@@ -1232,169 +1241,185 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B63" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B64" t="s">
+        <v>87</v>
+      </c>
+      <c r="C64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B65" t="s">
+        <v>88</v>
+      </c>
+      <c r="C65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B66" t="s">
         <v>89</v>
       </c>
-      <c r="C64" t="b">
+      <c r="C66" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A66" s="1" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A68" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B67" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B69" t="s">
         <v>91</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C69" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B68" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B70" t="s">
         <v>93</v>
       </c>
-      <c r="C68">
+      <c r="C70">
         <v>50</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>104</v>
-      </c>
-      <c r="B69" t="s">
-        <v>94</v>
-      </c>
-      <c r="C69">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
-        <v>24</v>
-      </c>
-      <c r="B70" t="s">
-        <v>95</v>
-      </c>
-      <c r="C70">
-        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>24</v>
+        <v>104</v>
       </c>
       <c r="B71" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B72" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C72">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B73" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C73">
-        <v>800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>108</v>
+        <v>16</v>
       </c>
       <c r="B74" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C74">
-        <v>8</v>
+        <v>500</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>108</v>
+        <v>16</v>
       </c>
       <c r="B75" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C75">
-        <v>8</v>
+        <v>800</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B76" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C76">
-        <v>8.0000000000000002E-3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B77" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C77">
-        <v>2000</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
+        <v>107</v>
+      </c>
+      <c r="B78" t="s">
+        <v>101</v>
+      </c>
+      <c r="C78">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>105</v>
+      </c>
+      <c r="B79" t="s">
+        <v>102</v>
+      </c>
+      <c r="C79">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
         <v>106</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B80" t="s">
         <v>103</v>
       </c>
-      <c r="C78">
+      <c r="C80">
         <v>4000</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A80" s="1" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A82" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B81" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B83" t="s">
         <v>110</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C83" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B82" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B84" t="s">
         <v>111</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C84" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Saves outputData to .mat file for each sim
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hombo\Documents\Github Repositories\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\Code of Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28844363-A925-4025-B7E6-57CC41F53D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EDEAE6-3BFF-4AB3-88C0-C67BB300FB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="117">
   <si>
     <t>dt</t>
   </si>
@@ -714,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -726,7 +726,7 @@
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -736,13 +736,16 @@
       <c r="C1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -752,8 +755,11 @@
       <c r="C4">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -763,8 +769,11 @@
       <c r="C5">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -774,8 +783,11 @@
       <c r="C6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -785,8 +797,11 @@
       <c r="C7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -796,8 +811,11 @@
       <c r="C8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -807,21 +825,27 @@
       <c r="C9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>116</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -831,8 +855,11 @@
       <c r="C13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -842,8 +869,11 @@
       <c r="C14">
         <v>2600</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D14">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -853,13 +883,16 @@
       <c r="C15">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -869,8 +902,11 @@
       <c r="C18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -880,8 +916,11 @@
       <c r="C19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -891,8 +930,11 @@
       <c r="C20" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -902,26 +944,32 @@
       <c r="C21">
         <v>9.81</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D21">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="2">
         <v>100000</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D25" s="2">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -931,21 +979,27 @@
       <c r="C26">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="2">
         <v>1000</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D28" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -955,21 +1009,27 @@
       <c r="C29">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D29">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>42</v>
       </c>
       <c r="C31">
         <v>3.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D31">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -979,8 +1039,11 @@
       <c r="C32">
         <v>-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D32">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -990,8 +1053,11 @@
       <c r="C33">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -1001,8 +1067,11 @@
       <c r="C34">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -1012,8 +1081,11 @@
       <c r="C35">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -1023,13 +1095,16 @@
       <c r="C36">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D36">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="1"/>
       <c r="B38" t="s">
         <v>54</v>
@@ -1037,21 +1112,27 @@
       <c r="C38" s="2">
         <v>2.0000000000000001E-4</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D38" s="2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
         <v>56</v>
       </c>
       <c r="C40">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D40">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>59</v>
       </c>
@@ -1061,13 +1142,16 @@
       <c r="C41" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>16</v>
       </c>
@@ -1077,8 +1161,11 @@
       <c r="C44">
         <v>1000</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D44">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>63</v>
       </c>
@@ -1088,8 +1175,11 @@
       <c r="C45">
         <v>5</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -1099,8 +1189,11 @@
       <c r="C46">
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>24</v>
       </c>
@@ -1110,8 +1203,11 @@
       <c r="C47">
         <v>15</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D47">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>67</v>
       </c>
@@ -1122,8 +1218,12 @@
         <f>-5/12*PI()</f>
         <v>-1.3089969389957472</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D48">
+        <f>-5/12*PI()</f>
+        <v>-1.3089969389957472</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>67</v>
       </c>
@@ -1134,8 +1234,12 @@
         <f>5/12*PI()</f>
         <v>1.3089969389957472</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D49">
+        <f>5/12*PI()</f>
+        <v>1.3089969389957472</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -1146,24 +1250,34 @@
         <f>11/6*PI()</f>
         <v>5.7595865315812871</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D50">
+        <f>11/6*PI()</f>
+        <v>5.7595865315812871</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B51" t="s">
         <v>71</v>
       </c>
       <c r="C51">
         <v>-1.8429999999999998E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D51">
+        <v>-1.8429999999999998E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
         <v>72</v>
       </c>
       <c r="C52">
         <v>0.37819999999999998</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D52">
+        <v>0.37819999999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B53" t="s">
         <v>73</v>
       </c>
@@ -1171,8 +1285,12 @@
         <f>-2.3782</f>
         <v>-2.3782000000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D53">
+        <f>-2.3782</f>
+        <v>-2.3782000000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -1182,37 +1300,49 @@
       <c r="C54">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
         <v>75</v>
       </c>
       <c r="C57" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D57" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B58" t="s">
         <v>77</v>
       </c>
       <c r="C58" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D58" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B59" t="s">
         <v>79</v>
       </c>
       <c r="C59" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D59" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>83</v>
       </c>
@@ -1222,77 +1352,104 @@
       <c r="C60" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
         <v>84</v>
       </c>
       <c r="C61" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D61" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B62" t="s">
         <v>85</v>
       </c>
       <c r="C62" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B63" t="s">
         <v>86</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B64" t="s">
         <v>87</v>
       </c>
       <c r="C64" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B65" t="s">
         <v>88</v>
       </c>
       <c r="C65" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B66" t="s">
         <v>89</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B69" t="s">
         <v>91</v>
       </c>
       <c r="C69" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D69" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B70" t="s">
         <v>93</v>
       </c>
       <c r="C70">
         <v>50</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D70">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>104</v>
       </c>
@@ -1302,8 +1459,11 @@
       <c r="C71">
         <v>50</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D71">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>24</v>
       </c>
@@ -1313,8 +1473,11 @@
       <c r="C72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>24</v>
       </c>
@@ -1324,8 +1487,11 @@
       <c r="C73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>16</v>
       </c>
@@ -1335,8 +1501,11 @@
       <c r="C74">
         <v>500</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D74">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -1346,8 +1515,11 @@
       <c r="C75">
         <v>800</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D75">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>108</v>
       </c>
@@ -1357,8 +1529,11 @@
       <c r="C76">
         <v>8</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D76">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>108</v>
       </c>
@@ -1368,8 +1543,11 @@
       <c r="C77">
         <v>8</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D77">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>107</v>
       </c>
@@ -1379,8 +1557,11 @@
       <c r="C78">
         <v>8.0000000000000002E-3</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D78">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>105</v>
       </c>
@@ -1390,8 +1571,11 @@
       <c r="C79">
         <v>2000</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D79">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>106</v>
       </c>
@@ -1401,25 +1585,34 @@
       <c r="C80">
         <v>4000</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D80">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B83" t="s">
         <v>110</v>
       </c>
       <c r="C83" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D83" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B84" t="s">
         <v>111</v>
       </c>
       <c r="C84" t="s">
+        <v>113</v>
+      </c>
+      <c r="D84" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tweaked agentControl_Adam. Small fixed for ThermalMap
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hombo\Documents\Github Repositories\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\Code of Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E9488F-122D-4110-96DB-CC135D1A2B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15183F3-A63C-4AE8-8743-C0A30E22DC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="144">
   <si>
     <t>dt</t>
   </si>
@@ -369,9 +369,6 @@
     <t>coh_relativeAscension</t>
   </si>
   <si>
-    <t>[0.5,4]</t>
-  </si>
-  <si>
     <t>[0,1]</t>
   </si>
   <si>
@@ -420,9 +417,6 @@
     <t>coh_heightDesire</t>
   </si>
   <si>
-    <t>[1,5]</t>
-  </si>
-  <si>
     <t>sep_relativeHeight</t>
   </si>
   <si>
@@ -457,6 +451,21 @@
   </si>
   <si>
     <t>neighborFrameSkip</t>
+  </si>
+  <si>
+    <t>[1,4]</t>
+  </si>
+  <si>
+    <t>[5,1]</t>
+  </si>
+  <si>
+    <t>Thermal Stuff</t>
+  </si>
+  <si>
+    <t>thermalBankFactor</t>
+  </si>
+  <si>
+    <t>Multiplier for thermal affected banking</t>
   </si>
 </sst>
 </file>
@@ -500,12 +509,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -786,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -798,7 +809,7 @@
     <col min="2" max="2" width="23.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -817,13 +828,25 @@
       <c r="F1">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -842,8 +865,20 @@
       <c r="F4">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G4">
+        <v>0.1</v>
+      </c>
+      <c r="H4">
+        <v>0.1</v>
+      </c>
+      <c r="I4">
+        <v>0.1</v>
+      </c>
+      <c r="J4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -862,8 +897,20 @@
       <c r="F5">
         <v>300</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G5">
+        <v>300</v>
+      </c>
+      <c r="H5">
+        <v>300</v>
+      </c>
+      <c r="I5">
+        <v>300</v>
+      </c>
+      <c r="J5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -871,19 +918,31 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
+      <c r="I6">
+        <v>30</v>
+      </c>
+      <c r="J6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -891,19 +950,31 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -922,8 +993,20 @@
       <c r="F8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8">
+        <v>20</v>
+      </c>
+      <c r="J8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -942,8 +1025,20 @@
       <c r="F9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>102</v>
       </c>
@@ -959,10 +1054,22 @@
       <c r="F10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -976,13 +1083,25 @@
       <c r="F11">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1001,8 +1120,20 @@
       <c r="F14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1021,8 +1152,20 @@
       <c r="F15">
         <v>2600</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G15">
+        <v>2600</v>
+      </c>
+      <c r="H15">
+        <v>2600</v>
+      </c>
+      <c r="I15">
+        <v>2600</v>
+      </c>
+      <c r="J15">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1041,13 +1184,25 @@
       <c r="F16">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1066,8 +1221,20 @@
       <c r="F19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1086,8 +1253,20 @@
       <c r="F20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" t="s">
+        <v>23</v>
+      </c>
+      <c r="J20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1106,8 +1285,20 @@
       <c r="F21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1126,390 +1317,604 @@
       <c r="F22">
         <v>9.81</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G22">
+        <v>9.81</v>
+      </c>
+      <c r="H22">
+        <v>9.81</v>
+      </c>
+      <c r="I22">
+        <v>9.81</v>
+      </c>
+      <c r="J22">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" t="s">
+        <v>139</v>
+      </c>
+      <c r="D26" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" t="s">
+        <v>139</v>
+      </c>
+      <c r="G26" t="s">
+        <v>139</v>
+      </c>
+      <c r="H26" t="s">
+        <v>139</v>
+      </c>
+      <c r="I26" t="s">
+        <v>139</v>
+      </c>
+      <c r="J26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>113</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>115</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>111</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>111</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>111</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>114</v>
-      </c>
-      <c r="B27" t="s">
-        <v>116</v>
-      </c>
-      <c r="C27" t="s">
-        <v>112</v>
-      </c>
-      <c r="D27" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" t="s">
-        <v>112</v>
-      </c>
-      <c r="F27" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G27" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" t="s">
+        <v>111</v>
+      </c>
+      <c r="I27" t="s">
+        <v>111</v>
+      </c>
+      <c r="J27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B30" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E30" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F30" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+        <v>137</v>
+      </c>
+      <c r="G30" t="s">
+        <v>137</v>
+      </c>
+      <c r="H30" t="s">
+        <v>137</v>
+      </c>
+      <c r="I30" t="s">
+        <v>137</v>
+      </c>
+      <c r="J30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B33" t="s">
         <v>117</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>118</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" t="s">
+        <v>118</v>
+      </c>
+      <c r="F33" t="s">
+        <v>118</v>
+      </c>
+      <c r="G33" t="s">
+        <v>118</v>
+      </c>
+      <c r="H33" t="s">
+        <v>118</v>
+      </c>
+      <c r="I33" t="s">
+        <v>118</v>
+      </c>
+      <c r="J33" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
         <v>119</v>
       </c>
-      <c r="D33" t="s">
-        <v>119</v>
-      </c>
-      <c r="E33" t="s">
-        <v>119</v>
-      </c>
-      <c r="F33" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
         <v>120</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>121</v>
       </c>
-      <c r="C34" t="s">
-        <v>122</v>
-      </c>
       <c r="D34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F34" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+        <v>121</v>
+      </c>
+      <c r="G34" t="s">
+        <v>121</v>
+      </c>
+      <c r="H34" t="s">
+        <v>121</v>
+      </c>
+      <c r="I34" t="s">
+        <v>121</v>
+      </c>
+      <c r="J34" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
         <v>38</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42">
         <v>2</v>
       </c>
       <c r="E42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+      <c r="G42">
+        <v>5</v>
+      </c>
+      <c r="H42">
+        <v>6</v>
+      </c>
+      <c r="I42">
+        <v>7</v>
+      </c>
+      <c r="J42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B43" t="s">
         <v>110</v>
       </c>
       <c r="C43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F43" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+      <c r="G43" t="s">
+        <v>122</v>
+      </c>
+      <c r="H43" t="s">
+        <v>122</v>
+      </c>
+      <c r="I43" t="s">
+        <v>122</v>
+      </c>
+      <c r="J43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44" t="s">
         <v>126</v>
       </c>
-      <c r="B44" t="s">
-        <v>127</v>
-      </c>
       <c r="C44" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="D44" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="E44" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="F44" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+        <v>140</v>
+      </c>
+      <c r="G44" t="s">
+        <v>140</v>
+      </c>
+      <c r="H44" t="s">
+        <v>140</v>
+      </c>
+      <c r="I44" t="s">
+        <v>140</v>
+      </c>
+      <c r="J44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="2">
-        <v>10</v>
-      </c>
-      <c r="D47" s="2">
-        <v>10</v>
-      </c>
-      <c r="E47" s="2">
-        <v>100</v>
-      </c>
-      <c r="F47" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="C47" s="6">
+        <v>20</v>
+      </c>
+      <c r="D47" s="6">
+        <v>20</v>
+      </c>
+      <c r="E47" s="6">
+        <v>20</v>
+      </c>
+      <c r="F47" s="6">
+        <v>20</v>
+      </c>
+      <c r="G47" s="6">
+        <v>20</v>
+      </c>
+      <c r="H47" s="6">
+        <v>20</v>
+      </c>
+      <c r="I47" s="6">
+        <v>20</v>
+      </c>
+      <c r="J47" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B48" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" t="s">
+        <v>128</v>
+      </c>
+      <c r="D48" t="s">
+        <v>128</v>
+      </c>
+      <c r="E48" t="s">
+        <v>128</v>
+      </c>
+      <c r="F48" t="s">
+        <v>128</v>
+      </c>
+      <c r="G48" t="s">
+        <v>128</v>
+      </c>
+      <c r="H48" t="s">
+        <v>128</v>
+      </c>
+      <c r="I48" t="s">
+        <v>128</v>
+      </c>
+      <c r="J48" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
         <v>129</v>
-      </c>
-      <c r="C48" t="s">
-        <v>130</v>
-      </c>
-      <c r="D48" t="s">
-        <v>130</v>
-      </c>
-      <c r="E48" t="s">
-        <v>130</v>
-      </c>
-      <c r="F48" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>131</v>
       </c>
       <c r="B49" t="s">
         <v>109</v>
       </c>
       <c r="C49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F49" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+      <c r="G49" t="s">
+        <v>122</v>
+      </c>
+      <c r="H49" t="s">
+        <v>122</v>
+      </c>
+      <c r="I49" t="s">
+        <v>122</v>
+      </c>
+      <c r="J49" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
         <v>36</v>
       </c>
       <c r="C52" s="2">
-        <v>10</v>
+        <v>0.2</v>
       </c>
       <c r="D52" s="2">
-        <v>10</v>
+        <v>0.2</v>
       </c>
       <c r="E52" s="2">
-        <v>100</v>
+        <v>0.2</v>
       </c>
       <c r="F52" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+        <v>0.2</v>
+      </c>
+      <c r="G52" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="J52" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
+        <v>130</v>
+      </c>
+      <c r="B53" t="s">
         <v>132</v>
       </c>
-      <c r="B53" t="s">
-        <v>134</v>
-      </c>
       <c r="C53" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D53" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E53" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F53" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+        <v>128</v>
+      </c>
+      <c r="G53" t="s">
+        <v>128</v>
+      </c>
+      <c r="H53" t="s">
+        <v>128</v>
+      </c>
+      <c r="I53" t="s">
+        <v>128</v>
+      </c>
+      <c r="J53" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54" t="s">
         <v>133</v>
       </c>
-      <c r="B54" t="s">
-        <v>135</v>
-      </c>
       <c r="C54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F54" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+        <v>122</v>
+      </c>
+      <c r="G54" t="s">
+        <v>122</v>
+      </c>
+      <c r="H54" t="s">
+        <v>122</v>
+      </c>
+      <c r="I54" t="s">
+        <v>122</v>
+      </c>
+      <c r="J54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A57" s="1"/>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A57" s="5">
+        <v>1E-8</v>
+      </c>
       <c r="B57" t="s">
         <v>40</v>
       </c>
       <c r="C57" s="2">
-        <v>1E-8</v>
+        <v>0</v>
       </c>
       <c r="D57" s="2">
-        <v>1E-8</v>
+        <v>0</v>
       </c>
       <c r="E57" s="2">
-        <v>1E-8</v>
+        <v>0</v>
       </c>
       <c r="F57" s="2">
-        <v>1E-8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="G57" s="2">
+        <v>0</v>
+      </c>
+      <c r="H57" s="2">
+        <v>0</v>
+      </c>
+      <c r="I57" s="2">
+        <v>0</v>
+      </c>
+      <c r="J57" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B58" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+        <v>111</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="1"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
         <v>42</v>
       </c>
@@ -1525,8 +1930,20 @@
       <c r="F61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
         <v>45</v>
       </c>
@@ -1545,692 +1962,1159 @@
       <c r="F62" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G62" t="s">
+        <v>44</v>
+      </c>
+      <c r="H62" t="s">
+        <v>44</v>
+      </c>
+      <c r="I62" t="s">
+        <v>44</v>
+      </c>
+      <c r="J62" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A65" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B65" t="s">
+        <v>142</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A67" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
         <v>16</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B68" t="s">
         <v>47</v>
       </c>
-      <c r="C65">
+      <c r="C68">
         <v>1000</v>
       </c>
-      <c r="D65">
+      <c r="D68">
         <v>1000</v>
       </c>
-      <c r="E65">
+      <c r="E68">
         <v>1000</v>
       </c>
-      <c r="F65">
+      <c r="F68">
         <v>1000</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
+      <c r="G68">
+        <v>1000</v>
+      </c>
+      <c r="H68">
+        <v>1000</v>
+      </c>
+      <c r="I68">
+        <v>1000</v>
+      </c>
+      <c r="J68">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
         <v>49</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B69" t="s">
         <v>48</v>
       </c>
-      <c r="C66">
+      <c r="C69">
         <v>5</v>
       </c>
-      <c r="D66">
+      <c r="D69">
         <v>5</v>
       </c>
-      <c r="E66">
+      <c r="E69">
         <v>5</v>
       </c>
-      <c r="F66">
+      <c r="F69">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
+      <c r="G69">
+        <v>5</v>
+      </c>
+      <c r="H69">
+        <v>5</v>
+      </c>
+      <c r="I69">
+        <v>5</v>
+      </c>
+      <c r="J69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
         <v>24</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B70" t="s">
         <v>50</v>
       </c>
-      <c r="C67">
+      <c r="C70">
         <v>5</v>
       </c>
-      <c r="D67">
+      <c r="D70">
         <v>5</v>
       </c>
-      <c r="E67">
+      <c r="E70">
         <v>5</v>
       </c>
-      <c r="F67">
+      <c r="F70">
         <v>5</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
+      <c r="G70">
+        <v>5</v>
+      </c>
+      <c r="H70">
+        <v>5</v>
+      </c>
+      <c r="I70">
+        <v>5</v>
+      </c>
+      <c r="J70">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
         <v>24</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B71" t="s">
         <v>51</v>
       </c>
-      <c r="C68">
+      <c r="C71">
         <v>15</v>
       </c>
-      <c r="D68">
+      <c r="D71">
         <v>15</v>
       </c>
-      <c r="E68">
+      <c r="E71">
         <v>15</v>
       </c>
-      <c r="F68">
+      <c r="F71">
         <v>15</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
+      <c r="G71">
+        <v>15</v>
+      </c>
+      <c r="H71">
+        <v>15</v>
+      </c>
+      <c r="I71">
+        <v>15</v>
+      </c>
+      <c r="J71">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
         <v>53</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B72" t="s">
         <v>52</v>
       </c>
-      <c r="C69">
-        <f>-5/12*PI()</f>
+      <c r="C72">
+        <f t="shared" ref="C72:J72" si="0">-5/12*PI()</f>
         <v>-1.3089969389957472</v>
       </c>
-      <c r="D69">
-        <f>-5/12*PI()</f>
+      <c r="D72">
+        <f t="shared" si="0"/>
         <v>-1.3089969389957472</v>
       </c>
-      <c r="E69">
-        <f>-5/12*PI()</f>
+      <c r="E72">
+        <f t="shared" si="0"/>
         <v>-1.3089969389957472</v>
       </c>
-      <c r="F69">
-        <f>-5/12*PI()</f>
+      <c r="F72">
+        <f t="shared" si="0"/>
         <v>-1.3089969389957472</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
+      <c r="G72">
+        <f t="shared" si="0"/>
+        <v>-1.3089969389957472</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="0"/>
+        <v>-1.3089969389957472</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="0"/>
+        <v>-1.3089969389957472</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="0"/>
+        <v>-1.3089969389957472</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
         <v>53</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B73" t="s">
         <v>54</v>
       </c>
-      <c r="C70">
-        <f>5/12*PI()</f>
+      <c r="C73">
+        <f t="shared" ref="C73:J73" si="1">5/12*PI()</f>
         <v>1.3089969389957472</v>
       </c>
-      <c r="D70">
-        <f>5/12*PI()</f>
+      <c r="D73">
+        <f t="shared" si="1"/>
         <v>1.3089969389957472</v>
       </c>
-      <c r="E70">
-        <f>5/12*PI()</f>
+      <c r="E73">
+        <f t="shared" si="1"/>
         <v>1.3089969389957472</v>
       </c>
-      <c r="F70">
-        <f>5/12*PI()</f>
+      <c r="F73">
+        <f t="shared" si="1"/>
         <v>1.3089969389957472</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
+      <c r="G73">
+        <f t="shared" si="1"/>
+        <v>1.3089969389957472</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="1"/>
+        <v>1.3089969389957472</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="1"/>
+        <v>1.3089969389957472</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="1"/>
+        <v>1.3089969389957472</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
         <v>56</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B74" t="s">
         <v>55</v>
       </c>
-      <c r="C71">
-        <f>11/6*PI()</f>
+      <c r="C74">
+        <f t="shared" ref="C74:J74" si="2">11/6*PI()</f>
         <v>5.7595865315812871</v>
       </c>
-      <c r="D71">
-        <f>11/6*PI()</f>
+      <c r="D74">
+        <f t="shared" si="2"/>
         <v>5.7595865315812871</v>
       </c>
-      <c r="E71">
-        <f>11/6*PI()</f>
+      <c r="E74">
+        <f t="shared" si="2"/>
         <v>5.7595865315812871</v>
       </c>
-      <c r="F71">
-        <f>11/6*PI()</f>
+      <c r="F74">
+        <f t="shared" si="2"/>
         <v>5.7595865315812871</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B72" t="s">
+      <c r="G74">
+        <f t="shared" si="2"/>
+        <v>5.7595865315812871</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="2"/>
+        <v>5.7595865315812871</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="2"/>
+        <v>5.7595865315812871</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="2"/>
+        <v>5.7595865315812871</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B75" t="s">
         <v>57</v>
       </c>
-      <c r="C72">
+      <c r="C75">
         <v>-1.8429999999999998E-2</v>
       </c>
-      <c r="D72">
+      <c r="D75">
         <v>-1.8429999999999998E-2</v>
       </c>
-      <c r="E72">
+      <c r="E75">
         <v>-1.8429999999999998E-2</v>
       </c>
-      <c r="F72">
+      <c r="F75">
         <v>-1.8429999999999998E-2</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B73" t="s">
+      <c r="G75">
+        <v>-1.8429999999999998E-2</v>
+      </c>
+      <c r="H75">
+        <v>-1.8429999999999998E-2</v>
+      </c>
+      <c r="I75">
+        <v>-1.8429999999999998E-2</v>
+      </c>
+      <c r="J75">
+        <v>-1.8429999999999998E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B76" t="s">
         <v>58</v>
       </c>
-      <c r="C73">
+      <c r="C76">
         <v>0.37819999999999998</v>
       </c>
-      <c r="D73">
+      <c r="D76">
         <v>0.37819999999999998</v>
       </c>
-      <c r="E73">
+      <c r="E76">
         <v>0.37819999999999998</v>
       </c>
-      <c r="F73">
+      <c r="F76">
         <v>0.37819999999999998</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B74" t="s">
+      <c r="G76">
+        <v>0.37819999999999998</v>
+      </c>
+      <c r="H76">
+        <v>0.37819999999999998</v>
+      </c>
+      <c r="I76">
+        <v>0.37819999999999998</v>
+      </c>
+      <c r="J76">
+        <v>0.37819999999999998</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B77" t="s">
         <v>59</v>
       </c>
-      <c r="C74">
-        <f>-2.3782</f>
+      <c r="C77">
+        <f t="shared" ref="C77:J77" si="3">-2.3782</f>
         <v>-2.3782000000000001</v>
       </c>
-      <c r="D74">
-        <f>-2.3782</f>
+      <c r="D77">
+        <f t="shared" si="3"/>
         <v>-2.3782000000000001</v>
       </c>
-      <c r="E74">
-        <f>-2.3782</f>
+      <c r="E77">
+        <f t="shared" si="3"/>
         <v>-2.3782000000000001</v>
       </c>
-      <c r="F74">
-        <f>-2.3782</f>
+      <c r="F77">
+        <f t="shared" si="3"/>
         <v>-2.3782000000000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
+      <c r="G77">
+        <f t="shared" si="3"/>
+        <v>-2.3782000000000001</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="3"/>
+        <v>-2.3782000000000001</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="3"/>
+        <v>-2.3782000000000001</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="3"/>
+        <v>-2.3782000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
         <v>16</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B78" t="s">
         <v>101</v>
       </c>
-      <c r="C75">
+      <c r="C78">
         <v>4</v>
       </c>
-      <c r="D75">
+      <c r="D78">
         <v>4</v>
       </c>
-      <c r="E75">
+      <c r="E78">
         <v>4</v>
       </c>
-      <c r="F75">
+      <c r="F78">
         <v>4</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A77" s="1" t="s">
+      <c r="G78">
+        <v>4</v>
+      </c>
+      <c r="H78">
+        <v>4</v>
+      </c>
+      <c r="I78">
+        <v>4</v>
+      </c>
+      <c r="J78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A80" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B78" t="s">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B81" t="s">
         <v>61</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C81" t="s">
         <v>62</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D81" t="s">
         <v>62</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E81" t="s">
         <v>62</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F81" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B79" t="s">
+      <c r="G81" t="s">
+        <v>62</v>
+      </c>
+      <c r="H81" t="s">
+        <v>62</v>
+      </c>
+      <c r="I81" t="s">
+        <v>62</v>
+      </c>
+      <c r="J81" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B82" t="s">
         <v>63</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C82" t="s">
         <v>64</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D82" t="s">
         <v>64</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E82" t="s">
         <v>64</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F82" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B80" t="s">
+      <c r="G82" t="s">
+        <v>64</v>
+      </c>
+      <c r="H82" t="s">
+        <v>64</v>
+      </c>
+      <c r="I82" t="s">
+        <v>64</v>
+      </c>
+      <c r="J82" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B83" t="s">
         <v>65</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C83" t="s">
         <v>66</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D83" t="s">
         <v>66</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E83" t="s">
         <v>66</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F83" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
+      <c r="G83" t="s">
+        <v>66</v>
+      </c>
+      <c r="H83" t="s">
+        <v>66</v>
+      </c>
+      <c r="I83" t="s">
+        <v>66</v>
+      </c>
+      <c r="J83" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
         <v>69</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B84" t="s">
         <v>67</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C84" t="s">
         <v>68</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D84" t="s">
         <v>68</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E84" t="s">
         <v>68</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F84" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B82" t="s">
+      <c r="G84" t="s">
+        <v>68</v>
+      </c>
+      <c r="H84" t="s">
+        <v>68</v>
+      </c>
+      <c r="I84" t="s">
+        <v>68</v>
+      </c>
+      <c r="J84" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B85" t="s">
         <v>70</v>
       </c>
-      <c r="C82" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D82" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F82" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B83" t="s">
+      <c r="C85" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D85" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F85" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G85" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H85" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I85" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J85" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B86" t="s">
         <v>71</v>
       </c>
-      <c r="C83" t="b">
-        <v>1</v>
-      </c>
-      <c r="D83" t="b">
-        <v>1</v>
-      </c>
-      <c r="E83" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B84" t="s">
+      <c r="C86" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86" t="b">
+        <v>1</v>
+      </c>
+      <c r="E86" t="b">
+        <v>1</v>
+      </c>
+      <c r="F86" t="b">
+        <v>1</v>
+      </c>
+      <c r="G86" t="b">
+        <v>1</v>
+      </c>
+      <c r="H86" t="b">
+        <v>1</v>
+      </c>
+      <c r="I86" t="b">
+        <v>1</v>
+      </c>
+      <c r="J86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B87" t="s">
         <v>72</v>
       </c>
-      <c r="C84" t="b">
-        <v>0</v>
-      </c>
-      <c r="D84" t="b">
-        <v>0</v>
-      </c>
-      <c r="E84" t="b">
-        <v>0</v>
-      </c>
-      <c r="F84" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B85" t="s">
+      <c r="C87" t="b">
+        <v>0</v>
+      </c>
+      <c r="D87" t="b">
+        <v>0</v>
+      </c>
+      <c r="E87" t="b">
+        <v>0</v>
+      </c>
+      <c r="F87" t="b">
+        <v>0</v>
+      </c>
+      <c r="G87" t="b">
+        <v>0</v>
+      </c>
+      <c r="H87" t="b">
+        <v>0</v>
+      </c>
+      <c r="I87" t="b">
+        <v>0</v>
+      </c>
+      <c r="J87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B88" t="s">
         <v>73</v>
       </c>
-      <c r="C85" t="b">
-        <v>1</v>
-      </c>
-      <c r="D85" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" t="b">
-        <v>1</v>
-      </c>
-      <c r="F85" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B86" t="s">
+      <c r="C88" t="b">
+        <v>1</v>
+      </c>
+      <c r="D88" t="b">
+        <v>1</v>
+      </c>
+      <c r="E88" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" t="b">
+        <v>1</v>
+      </c>
+      <c r="G88" t="b">
+        <v>1</v>
+      </c>
+      <c r="H88" t="b">
+        <v>1</v>
+      </c>
+      <c r="I88" t="b">
+        <v>1</v>
+      </c>
+      <c r="J88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B89" t="s">
         <v>74</v>
       </c>
-      <c r="C86" t="b">
-        <v>1</v>
-      </c>
-      <c r="D86" t="b">
-        <v>1</v>
-      </c>
-      <c r="E86" t="b">
-        <v>1</v>
-      </c>
-      <c r="F86" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B87" t="s">
+      <c r="C89" t="b">
+        <v>1</v>
+      </c>
+      <c r="D89" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" t="b">
+        <v>1</v>
+      </c>
+      <c r="G89" t="b">
+        <v>1</v>
+      </c>
+      <c r="H89" t="b">
+        <v>1</v>
+      </c>
+      <c r="I89" t="b">
+        <v>1</v>
+      </c>
+      <c r="J89" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B90" t="s">
         <v>75</v>
       </c>
-      <c r="C87" t="b">
-        <v>0</v>
-      </c>
-      <c r="D87" t="b">
-        <v>0</v>
-      </c>
-      <c r="E87" t="b">
-        <v>0</v>
-      </c>
-      <c r="F87" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A89" s="1" t="s">
+      <c r="C90" t="b">
+        <v>0</v>
+      </c>
+      <c r="D90" t="b">
+        <v>0</v>
+      </c>
+      <c r="E90" t="b">
+        <v>0</v>
+      </c>
+      <c r="F90" t="b">
+        <v>0</v>
+      </c>
+      <c r="G90" t="b">
+        <v>0</v>
+      </c>
+      <c r="H90" t="b">
+        <v>0</v>
+      </c>
+      <c r="I90" t="b">
+        <v>0</v>
+      </c>
+      <c r="J90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A92" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B90" t="s">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B93" t="s">
         <v>77</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C93" t="s">
         <v>78</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D93" t="s">
         <v>78</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E93" t="s">
         <v>78</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F93" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B91" t="s">
+      <c r="G93" t="s">
+        <v>78</v>
+      </c>
+      <c r="H93" t="s">
+        <v>78</v>
+      </c>
+      <c r="I93" t="s">
+        <v>78</v>
+      </c>
+      <c r="J93" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B94" t="s">
         <v>79</v>
       </c>
-      <c r="C91">
+      <c r="C94">
         <v>50</v>
       </c>
-      <c r="D91">
+      <c r="D94">
         <v>50</v>
       </c>
-      <c r="E91">
+      <c r="E94">
         <v>50</v>
       </c>
-      <c r="F91">
+      <c r="F94">
         <v>50</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A92" t="s">
+      <c r="G94">
+        <v>50</v>
+      </c>
+      <c r="H94">
+        <v>50</v>
+      </c>
+      <c r="I94">
+        <v>50</v>
+      </c>
+      <c r="J94">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
         <v>90</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B95" t="s">
         <v>80</v>
       </c>
-      <c r="C92">
+      <c r="C95">
         <v>50</v>
       </c>
-      <c r="D92">
+      <c r="D95">
         <v>50</v>
       </c>
-      <c r="E92">
+      <c r="E95">
         <v>50</v>
       </c>
-      <c r="F92">
+      <c r="F95">
         <v>50</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A93" t="s">
+      <c r="G95">
+        <v>50</v>
+      </c>
+      <c r="H95">
+        <v>50</v>
+      </c>
+      <c r="I95">
+        <v>50</v>
+      </c>
+      <c r="J95">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A96" t="s">
         <v>24</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B96" t="s">
         <v>81</v>
       </c>
-      <c r="C93">
-        <v>0</v>
-      </c>
-      <c r="D93">
-        <v>0</v>
-      </c>
-      <c r="E93">
-        <v>0</v>
-      </c>
-      <c r="F93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A94" t="s">
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96">
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A97" t="s">
         <v>24</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B97" t="s">
         <v>82</v>
       </c>
-      <c r="C94">
-        <v>0</v>
-      </c>
-      <c r="D94">
-        <v>0</v>
-      </c>
-      <c r="E94">
-        <v>0</v>
-      </c>
-      <c r="F94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A95" t="s">
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A98" t="s">
         <v>16</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B98" t="s">
         <v>83</v>
       </c>
-      <c r="C95">
+      <c r="C98">
         <v>500</v>
       </c>
-      <c r="D95">
+      <c r="D98">
         <v>500</v>
       </c>
-      <c r="E95">
+      <c r="E98">
         <v>500</v>
       </c>
-      <c r="F95">
+      <c r="F98">
         <v>500</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A96" t="s">
+      <c r="G98">
+        <v>500</v>
+      </c>
+      <c r="H98">
+        <v>500</v>
+      </c>
+      <c r="I98">
+        <v>500</v>
+      </c>
+      <c r="J98">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
         <v>16</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B99" t="s">
         <v>84</v>
       </c>
-      <c r="C96">
+      <c r="C99">
         <v>800</v>
       </c>
-      <c r="D96">
+      <c r="D99">
         <v>800</v>
       </c>
-      <c r="E96">
+      <c r="E99">
         <v>800</v>
       </c>
-      <c r="F96">
+      <c r="F99">
         <v>800</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A97" t="s">
+      <c r="G99">
+        <v>800</v>
+      </c>
+      <c r="H99">
+        <v>800</v>
+      </c>
+      <c r="I99">
+        <v>800</v>
+      </c>
+      <c r="J99">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
         <v>94</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B100" t="s">
         <v>85</v>
       </c>
-      <c r="C97">
+      <c r="C100">
         <v>8</v>
       </c>
-      <c r="D97">
+      <c r="D100">
         <v>8</v>
       </c>
-      <c r="E97">
+      <c r="E100">
         <v>8</v>
       </c>
-      <c r="F97">
+      <c r="F100">
         <v>8</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A98" t="s">
+      <c r="G100">
+        <v>8</v>
+      </c>
+      <c r="H100">
+        <v>8</v>
+      </c>
+      <c r="I100">
+        <v>8</v>
+      </c>
+      <c r="J100">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
         <v>94</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B101" t="s">
         <v>86</v>
       </c>
-      <c r="C98">
+      <c r="C101">
         <v>8</v>
       </c>
-      <c r="D98">
+      <c r="D101">
         <v>8</v>
       </c>
-      <c r="E98">
+      <c r="E101">
         <v>8</v>
       </c>
-      <c r="F98">
+      <c r="F101">
         <v>8</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A99" t="s">
+      <c r="G101">
+        <v>8</v>
+      </c>
+      <c r="H101">
+        <v>8</v>
+      </c>
+      <c r="I101">
+        <v>8</v>
+      </c>
+      <c r="J101">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
         <v>93</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B102" t="s">
         <v>87</v>
       </c>
-      <c r="C99">
+      <c r="C102">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D99">
+      <c r="D102">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="E99">
+      <c r="E102">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F99">
+      <c r="F102">
         <v>8.0000000000000002E-3</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A100" t="s">
+      <c r="G102">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H102">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I102">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="J102">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
         <v>91</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B103" t="s">
         <v>88</v>
       </c>
-      <c r="C100">
+      <c r="C103">
         <v>2000</v>
       </c>
-      <c r="D100">
+      <c r="D103">
         <v>2000</v>
       </c>
-      <c r="E100">
+      <c r="E103">
         <v>2000</v>
       </c>
-      <c r="F100">
+      <c r="F103">
         <v>2000</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A101" t="s">
+      <c r="G103">
+        <v>2000</v>
+      </c>
+      <c r="H103">
+        <v>2000</v>
+      </c>
+      <c r="I103">
+        <v>2000</v>
+      </c>
+      <c r="J103">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
         <v>92</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B104" t="s">
         <v>89</v>
       </c>
-      <c r="C101">
+      <c r="C104">
         <v>4000</v>
       </c>
-      <c r="D101">
+      <c r="D104">
         <v>4000</v>
       </c>
-      <c r="E101">
+      <c r="E104">
         <v>4000</v>
       </c>
-      <c r="F101">
+      <c r="F104">
         <v>4000</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A103" s="1" t="s">
+      <c r="G104">
+        <v>4000</v>
+      </c>
+      <c r="H104">
+        <v>4000</v>
+      </c>
+      <c r="I104">
+        <v>4000</v>
+      </c>
+      <c r="J104">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A106" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B104" t="s">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B107" t="s">
         <v>96</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C107" t="s">
         <v>98</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D107" t="s">
         <v>98</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E107" t="s">
         <v>98</v>
       </c>
-      <c r="F104" t="s">
+      <c r="F107" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="B105" t="s">
+      <c r="G107" t="s">
+        <v>98</v>
+      </c>
+      <c r="H107" t="s">
+        <v>98</v>
+      </c>
+      <c r="I107" t="s">
+        <v>98</v>
+      </c>
+      <c r="J107" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B108" t="s">
         <v>97</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C108" t="s">
         <v>99</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D108" t="s">
         <v>99</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E108" t="s">
         <v>99</v>
       </c>
-      <c r="F105" t="s">
+      <c r="F108" t="s">
+        <v>99</v>
+      </c>
+      <c r="G108" t="s">
+        <v>99</v>
+      </c>
+      <c r="H108" t="s">
+        <v>99</v>
+      </c>
+      <c r="I108" t="s">
+        <v>99</v>
+      </c>
+      <c r="J108" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AdamsLaw with RNG Test
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hombo\Documents\Github Repositories\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\Code of Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D7B84C-FA2E-4732-A928-0F436231937B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6117070E-D8B7-495A-B349-0A4138FD1544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="158">
   <si>
     <t>dt</t>
   </si>
@@ -499,6 +499,15 @@
   </si>
   <si>
     <t>listNeighborData</t>
+  </si>
+  <si>
+    <t>[1500,1500]</t>
+  </si>
+  <si>
+    <t>[1,4]</t>
+  </si>
+  <si>
+    <t>[0.66,1.33]</t>
   </si>
 </sst>
 </file>
@@ -830,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K117"/>
+  <dimension ref="A1:L117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -842,7 +851,7 @@
     <col min="2" max="2" width="23.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -852,37 +861,13 @@
       <c r="C1">
         <v>1</v>
       </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-      <c r="F1">
-        <v>1</v>
-      </c>
-      <c r="G1">
-        <v>1</v>
-      </c>
-      <c r="H1">
-        <v>1</v>
-      </c>
-      <c r="I1">
-        <v>1</v>
-      </c>
-      <c r="J1">
-        <v>1</v>
-      </c>
-      <c r="K1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -916,8 +901,11 @@
       <c r="K4">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -951,8 +939,11 @@
       <c r="K5">
         <v>300</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -986,8 +977,11 @@
       <c r="K6">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -995,7 +989,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D7">
         <v>20</v>
@@ -1021,8 +1015,11 @@
       <c r="K7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1056,8 +1053,11 @@
       <c r="K8">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1091,8 +1091,11 @@
       <c r="K9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>101</v>
       </c>
@@ -1123,8 +1126,11 @@
       <c r="K10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>135</v>
       </c>
@@ -1155,8 +1161,11 @@
       <c r="K11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>145</v>
       </c>
@@ -1187,8 +1196,11 @@
       <c r="K12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>146</v>
       </c>
@@ -1219,13 +1231,16 @@
       <c r="K13">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1259,8 +1274,11 @@
       <c r="K16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1294,8 +1312,11 @@
       <c r="K17">
         <v>2600</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L17">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1329,13 +1350,16 @@
       <c r="K18">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1369,8 +1393,11 @@
       <c r="K21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1378,7 +1405,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>155</v>
       </c>
       <c r="D22" t="s">
         <v>117</v>
@@ -1404,8 +1431,11 @@
       <c r="K22" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L22" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1439,8 +1469,11 @@
       <c r="K23" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1474,18 +1507,21 @@
       <c r="K24">
         <v>9.81</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L24">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>111</v>
       </c>
@@ -1519,8 +1555,11 @@
       <c r="K28" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -1554,13 +1593,16 @@
       <c r="K29" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -1594,13 +1636,16 @@
       <c r="K32" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>115</v>
       </c>
@@ -1608,7 +1653,7 @@
         <v>116</v>
       </c>
       <c r="C35" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="D35" t="s">
         <v>150</v>
@@ -1634,8 +1679,11 @@
       <c r="K35" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>118</v>
       </c>
@@ -1669,28 +1717,31 @@
       <c r="K36" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L36" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
         <v>37</v>
       </c>
@@ -1721,8 +1772,11 @@
       <c r="K44">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>121</v>
       </c>
@@ -1730,34 +1784,37 @@
         <v>109</v>
       </c>
       <c r="C45" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" t="s">
         <v>151</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>152</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>153</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>151</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>152</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>153</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
         <v>151</v>
       </c>
-      <c r="J45" t="s">
+      <c r="K45" t="s">
         <v>152</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>123</v>
       </c>
@@ -1791,8 +1848,11 @@
       <c r="K46" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>149</v>
       </c>
@@ -1826,17 +1886,20 @@
       <c r="K47">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="6">
+      <c r="C50">
         <v>20</v>
       </c>
       <c r="D50" s="6">
@@ -1846,7 +1909,7 @@
         <v>20</v>
       </c>
       <c r="F50" s="6">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G50" s="6">
         <v>30</v>
@@ -1855,7 +1918,7 @@
         <v>30</v>
       </c>
       <c r="I50" s="6">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="J50" s="6">
         <v>40</v>
@@ -1863,8 +1926,11 @@
       <c r="K50" s="6">
         <v>40</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L50" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>122</v>
       </c>
@@ -1898,8 +1964,11 @@
       <c r="K51" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L51" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>126</v>
       </c>
@@ -1907,7 +1976,7 @@
         <v>108</v>
       </c>
       <c r="C52" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="D52" t="s">
         <v>143</v>
@@ -1933,8 +2002,11 @@
       <c r="K52" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L52" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>140</v>
       </c>
@@ -1968,17 +2040,20 @@
       <c r="K53">
         <v>2000</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L53">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
         <v>35</v>
       </c>
-      <c r="C56" s="6">
+      <c r="C56">
         <v>2</v>
       </c>
       <c r="D56" s="6">
@@ -2005,8 +2080,11 @@
       <c r="K56" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L56" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>127</v>
       </c>
@@ -2040,8 +2118,11 @@
       <c r="K57" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L57" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>128</v>
       </c>
@@ -2049,7 +2130,7 @@
         <v>130</v>
       </c>
       <c r="C58" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="D58" t="s">
         <v>143</v>
@@ -2075,18 +2156,21 @@
       <c r="K58" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L58" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
         <v>142</v>
       </c>
       <c r="C61">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D61">
         <v>6</v>
@@ -2112,9 +2196,11 @@
       <c r="K61">
         <v>6</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C62" s="2"/>
+      <c r="L61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
@@ -2123,20 +2209,21 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A64" s="5">
         <v>1E-8</v>
       </c>
       <c r="B64" t="s">
         <v>39</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64">
         <v>0</v>
       </c>
       <c r="D64" s="2">
@@ -2163,15 +2250,18 @@
       <c r="K64" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L64" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B65" t="s">
         <v>132</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" t="s">
         <v>110</v>
       </c>
       <c r="D65" s="2" t="s">
@@ -2198,10 +2288,12 @@
       <c r="K65" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L65" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A66" s="1"/>
-      <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
@@ -2210,13 +2302,14 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B68" t="s">
         <v>41</v>
       </c>
@@ -2247,8 +2340,11 @@
       <c r="K68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
         <v>44</v>
       </c>
@@ -2282,16 +2378,19 @@
       <c r="K69" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L69" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A70" s="3"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
         <v>138</v>
       </c>
@@ -2325,13 +2424,16 @@
       <c r="K72">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -2365,8 +2467,11 @@
       <c r="K75">
         <v>1000</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L75">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -2400,8 +2505,11 @@
       <c r="K76">
         <v>5</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L76">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>23</v>
       </c>
@@ -2435,8 +2543,11 @@
       <c r="K77">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>23</v>
       </c>
@@ -2470,8 +2581,11 @@
       <c r="K78">
         <v>15</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L78">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>52</v>
       </c>
@@ -2479,11 +2593,10 @@
         <v>51</v>
       </c>
       <c r="C79">
-        <f t="shared" ref="C79:K79" si="0">-5/12*PI()</f>
         <v>-1.3089969389957472</v>
       </c>
       <c r="D79">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D79:L79" si="0">-5/12*PI()</f>
         <v>-1.3089969389957472</v>
       </c>
       <c r="E79">
@@ -2514,8 +2627,12 @@
         <f t="shared" si="0"/>
         <v>-1.3089969389957472</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L79">
+        <f t="shared" si="0"/>
+        <v>-1.3089969389957472</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>52</v>
       </c>
@@ -2523,11 +2640,10 @@
         <v>53</v>
       </c>
       <c r="C80">
-        <f t="shared" ref="C80:K80" si="1">5/12*PI()</f>
         <v>1.3089969389957472</v>
       </c>
       <c r="D80">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D80:L80" si="1">5/12*PI()</f>
         <v>1.3089969389957472</v>
       </c>
       <c r="E80">
@@ -2558,8 +2674,12 @@
         <f t="shared" si="1"/>
         <v>1.3089969389957472</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L80">
+        <f t="shared" si="1"/>
+        <v>1.3089969389957472</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>55</v>
       </c>
@@ -2567,11 +2687,10 @@
         <v>54</v>
       </c>
       <c r="C81">
-        <f t="shared" ref="C81:K81" si="2">11/6*PI()</f>
         <v>5.7595865315812871</v>
       </c>
       <c r="D81">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D81:L81" si="2">11/6*PI()</f>
         <v>5.7595865315812871</v>
       </c>
       <c r="E81">
@@ -2602,8 +2721,12 @@
         <f t="shared" si="2"/>
         <v>5.7595865315812871</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L81">
+        <f t="shared" si="2"/>
+        <v>5.7595865315812871</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B82" t="s">
         <v>56</v>
       </c>
@@ -2634,8 +2757,11 @@
       <c r="K82">
         <v>-1.8429999999999998E-2</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L82">
+        <v>-1.8429999999999998E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B83" t="s">
         <v>57</v>
       </c>
@@ -2666,17 +2792,19 @@
       <c r="K83">
         <v>0.37819999999999998</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L83">
+        <v>0.37819999999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B84" t="s">
         <v>58</v>
       </c>
       <c r="C84">
-        <f t="shared" ref="C84:K84" si="3">-2.3782</f>
         <v>-2.3782000000000001</v>
       </c>
       <c r="D84">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D84:L84" si="3">-2.3782</f>
         <v>-2.3782000000000001</v>
       </c>
       <c r="E84">
@@ -2707,8 +2835,12 @@
         <f t="shared" si="3"/>
         <v>-2.3782000000000001</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L84">
+        <f t="shared" si="3"/>
+        <v>-2.3782000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -2742,13 +2874,16 @@
       <c r="K85">
         <v>4</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B88" t="s">
         <v>60</v>
       </c>
@@ -2779,8 +2914,11 @@
       <c r="K88" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L88" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B89" t="s">
         <v>62</v>
       </c>
@@ -2811,8 +2949,11 @@
       <c r="K89" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L89" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B90" t="s">
         <v>64</v>
       </c>
@@ -2843,8 +2984,11 @@
       <c r="K90" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L90" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>68</v>
       </c>
@@ -2878,12 +3022,15 @@
       <c r="K91" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L91" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B92" t="s">
         <v>69</v>
       </c>
-      <c r="C92" s="4" t="b">
+      <c r="C92" t="b">
         <v>1</v>
       </c>
       <c r="D92" s="4" t="b">
@@ -2910,8 +3057,11 @@
       <c r="K92" s="4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L92" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B93" t="s">
         <v>70</v>
       </c>
@@ -2942,8 +3092,11 @@
       <c r="K93" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B94" t="s">
         <v>71</v>
       </c>
@@ -2974,8 +3127,11 @@
       <c r="K94" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B95" t="s">
         <v>72</v>
       </c>
@@ -3006,8 +3162,11 @@
       <c r="K95" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L95" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B96" t="s">
         <v>73</v>
       </c>
@@ -3038,8 +3197,11 @@
       <c r="K96" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B97" t="s">
         <v>74</v>
       </c>
@@ -3070,8 +3232,11 @@
       <c r="K97" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B98" t="s">
         <v>147</v>
       </c>
@@ -3102,8 +3267,11 @@
       <c r="K98" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B99" t="s">
         <v>154</v>
       </c>
@@ -3134,13 +3302,16 @@
       <c r="K99" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B102" t="s">
         <v>76</v>
       </c>
@@ -3171,8 +3342,11 @@
       <c r="K102" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L102" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B103" t="s">
         <v>78</v>
       </c>
@@ -3203,8 +3377,11 @@
       <c r="K103">
         <v>50</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L103">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>89</v>
       </c>
@@ -3238,8 +3415,11 @@
       <c r="K104">
         <v>50</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L104">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>23</v>
       </c>
@@ -3273,8 +3453,11 @@
       <c r="K105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>23</v>
       </c>
@@ -3308,8 +3491,11 @@
       <c r="K106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>16</v>
       </c>
@@ -3343,8 +3529,11 @@
       <c r="K107">
         <v>500</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L107">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>16</v>
       </c>
@@ -3378,8 +3567,11 @@
       <c r="K108">
         <v>800</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L108">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>93</v>
       </c>
@@ -3413,8 +3605,11 @@
       <c r="K109">
         <v>8</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L109">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>93</v>
       </c>
@@ -3448,8 +3643,11 @@
       <c r="K110">
         <v>8</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L110">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>92</v>
       </c>
@@ -3483,8 +3681,11 @@
       <c r="K111">
         <v>8.0000000000000002E-3</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L111">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>90</v>
       </c>
@@ -3518,8 +3719,11 @@
       <c r="K112">
         <v>2000</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L112">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>91</v>
       </c>
@@ -3553,13 +3757,16 @@
       <c r="K113">
         <v>4000</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L113">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B116" t="s">
         <v>95</v>
       </c>
@@ -3590,8 +3797,11 @@
       <c r="K116" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="L116" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B117" t="s">
         <v>96</v>
       </c>
@@ -3620,6 +3830,9 @@
         <v>98</v>
       </c>
       <c r="K117" t="s">
+        <v>98</v>
+      </c>
+      <c r="L117" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Massive speed improvements to agentControl_Adam
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hombo\Documents\Github Repositories\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\Code of Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6117070E-D8B7-495A-B349-0A4138FD1544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762BB8DC-B40B-48B6-BAF0-C3447A44778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="155">
   <si>
     <t>dt</t>
   </si>
@@ -468,9 +468,6 @@
     <t>[1,1]</t>
   </si>
   <si>
-    <t>[1,16]</t>
-  </si>
-  <si>
     <t>render</t>
   </si>
   <si>
@@ -501,13 +498,7 @@
     <t>listNeighborData</t>
   </si>
   <si>
-    <t>[1500,1500]</t>
-  </si>
-  <si>
     <t>[1,4]</t>
-  </si>
-  <si>
-    <t>[0.66,1.33]</t>
   </si>
 </sst>
 </file>
@@ -839,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L117"/>
+  <dimension ref="A1:K117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -851,7 +842,7 @@
     <col min="2" max="2" width="23.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -861,13 +852,37 @@
       <c r="C1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+      <c r="J1">
+        <v>8</v>
+      </c>
+      <c r="K1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -901,11 +916,8 @@
       <c r="K4">
         <v>0.1</v>
       </c>
-      <c r="L4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -913,37 +925,34 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>300</v>
+        <v>1800</v>
       </c>
       <c r="D5">
-        <v>300</v>
+        <v>1800</v>
       </c>
       <c r="E5">
-        <v>300</v>
+        <v>1800</v>
       </c>
       <c r="F5">
-        <v>300</v>
+        <v>1800</v>
       </c>
       <c r="G5">
-        <v>300</v>
+        <v>1800</v>
       </c>
       <c r="H5">
-        <v>300</v>
+        <v>1800</v>
       </c>
       <c r="I5">
-        <v>300</v>
+        <v>1800</v>
       </c>
       <c r="J5">
-        <v>300</v>
+        <v>1800</v>
       </c>
       <c r="K5">
-        <v>300</v>
-      </c>
-      <c r="L5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -977,11 +986,8 @@
       <c r="K6">
         <v>30</v>
       </c>
-      <c r="L6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -989,37 +995,34 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D7">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E7">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F7">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="G7">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H7">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="I7">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="J7">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="K7">
-        <v>20</v>
-      </c>
-      <c r="L7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1053,11 +1056,8 @@
       <c r="K8">
         <v>40</v>
       </c>
-      <c r="L8">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1091,11 +1091,8 @@
       <c r="K9">
         <v>5</v>
       </c>
-      <c r="L9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>101</v>
       </c>
@@ -1126,121 +1123,109 @@
       <c r="K10" t="b">
         <v>1</v>
       </c>
-      <c r="L10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>135</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
         <v>145</v>
       </c>
-      <c r="C12" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" t="b">
-        <v>1</v>
-      </c>
-      <c r="L12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
-        <v>146</v>
-      </c>
       <c r="C13">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="D13">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="J13">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="K13">
-        <v>100</v>
-      </c>
-      <c r="L13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1274,11 +1259,8 @@
       <c r="K16" t="s">
         <v>14</v>
       </c>
-      <c r="L16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1312,11 +1294,8 @@
       <c r="K17">
         <v>2600</v>
       </c>
-      <c r="L17">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1350,16 +1329,13 @@
       <c r="K18">
         <v>0</v>
       </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1393,11 +1369,8 @@
       <c r="K21" t="s">
         <v>21</v>
       </c>
-      <c r="L21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1405,7 +1378,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>155</v>
+        <v>117</v>
       </c>
       <c r="D22" t="s">
         <v>117</v>
@@ -1431,11 +1404,8 @@
       <c r="K22" t="s">
         <v>117</v>
       </c>
-      <c r="L22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1469,11 +1439,8 @@
       <c r="K23" t="s">
         <v>25</v>
       </c>
-      <c r="L23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1507,21 +1474,18 @@
       <c r="K24">
         <v>9.81</v>
       </c>
-      <c r="L24">
-        <v>9.81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>111</v>
       </c>
@@ -1529,37 +1493,34 @@
         <v>113</v>
       </c>
       <c r="C28" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="D28" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="E28" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="F28" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="G28" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="H28" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="I28" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="J28" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="K28" t="s">
-        <v>144</v>
-      </c>
-      <c r="L28" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -1593,16 +1554,13 @@
       <c r="K29" t="s">
         <v>110</v>
       </c>
-      <c r="L29" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -1636,16 +1594,13 @@
       <c r="K32" t="s">
         <v>134</v>
       </c>
-      <c r="L32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>115</v>
       </c>
@@ -1653,37 +1608,34 @@
         <v>116</v>
       </c>
       <c r="C35" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="D35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K35" t="s">
-        <v>150</v>
-      </c>
-      <c r="L35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>118</v>
       </c>
@@ -1717,31 +1669,28 @@
       <c r="K36" t="s">
         <v>120</v>
       </c>
-      <c r="L36" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
         <v>37</v>
       </c>
@@ -1772,11 +1721,8 @@
       <c r="K44">
         <v>4</v>
       </c>
-      <c r="L44">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>121</v>
       </c>
@@ -1784,7 +1730,7 @@
         <v>109</v>
       </c>
       <c r="C45" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D45" t="s">
         <v>151</v>
@@ -1793,7 +1739,7 @@
         <v>152</v>
       </c>
       <c r="F45" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G45" t="s">
         <v>151</v>
@@ -1802,7 +1748,7 @@
         <v>152</v>
       </c>
       <c r="I45" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J45" t="s">
         <v>151</v>
@@ -1810,11 +1756,8 @@
       <c r="K45" t="s">
         <v>152</v>
       </c>
-      <c r="L45" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>123</v>
       </c>
@@ -1848,16 +1791,13 @@
       <c r="K46" t="s">
         <v>143</v>
       </c>
-      <c r="L46" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1886,30 +1826,27 @@
       <c r="K47">
         <v>0</v>
       </c>
-      <c r="L47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
         <v>33</v>
       </c>
-      <c r="C50">
-        <v>20</v>
+      <c r="C50" s="6">
+        <v>4</v>
       </c>
       <c r="D50" s="6">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="E50" s="6">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F50" s="6">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G50" s="6">
         <v>30</v>
@@ -1918,19 +1855,16 @@
         <v>30</v>
       </c>
       <c r="I50" s="6">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="J50" s="6">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="K50" s="6">
-        <v>40</v>
-      </c>
-      <c r="L50" s="6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>122</v>
       </c>
@@ -1964,11 +1898,8 @@
       <c r="K51" t="s">
         <v>143</v>
       </c>
-      <c r="L51" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>126</v>
       </c>
@@ -1976,7 +1907,7 @@
         <v>108</v>
       </c>
       <c r="C52" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="D52" t="s">
         <v>143</v>
@@ -2002,11 +1933,8 @@
       <c r="K52" t="s">
         <v>143</v>
       </c>
-      <c r="L52" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>140</v>
       </c>
@@ -2040,51 +1968,45 @@
       <c r="K53">
         <v>2000</v>
       </c>
-      <c r="L53">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
         <v>35</v>
       </c>
-      <c r="C56">
-        <v>2</v>
+      <c r="C56" s="6">
+        <v>0.2</v>
       </c>
       <c r="D56" s="6">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="E56" s="6">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="F56" s="6">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="G56" s="6">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="H56" s="6">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="I56" s="6">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="J56" s="6">
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="K56" s="6">
-        <v>2</v>
-      </c>
-      <c r="L56" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>127</v>
       </c>
@@ -2118,11 +2040,8 @@
       <c r="K57" t="s">
         <v>143</v>
       </c>
-      <c r="L57" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>128</v>
       </c>
@@ -2130,7 +2049,7 @@
         <v>130</v>
       </c>
       <c r="C58" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="D58" t="s">
         <v>143</v>
@@ -2156,21 +2075,18 @@
       <c r="K58" t="s">
         <v>143</v>
       </c>
-      <c r="L58" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
         <v>142</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D61">
         <v>6</v>
@@ -2196,11 +2112,9 @@
       <c r="K61">
         <v>6</v>
       </c>
-      <c r="L61">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
@@ -2209,21 +2123,20 @@
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" s="5">
         <v>1E-8</v>
       </c>
       <c r="B64" t="s">
         <v>39</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="2">
         <v>0</v>
       </c>
       <c r="D64" s="2">
@@ -2250,18 +2163,15 @@
       <c r="K64" s="2">
         <v>0</v>
       </c>
-      <c r="L64" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
         <v>131</v>
       </c>
       <c r="B65" t="s">
         <v>132</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="2" t="s">
         <v>110</v>
       </c>
       <c r="D65" s="2" t="s">
@@ -2288,12 +2198,10 @@
       <c r="K65" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="L65" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66" s="1"/>
+      <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
@@ -2302,14 +2210,13 @@
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
-      <c r="L66" s="2"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B68" t="s">
         <v>41</v>
       </c>
@@ -2340,11 +2247,8 @@
       <c r="K68">
         <v>0</v>
       </c>
-      <c r="L68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" s="3" t="s">
         <v>44</v>
       </c>
@@ -2378,19 +2282,16 @@
       <c r="K69" t="s">
         <v>43</v>
       </c>
-      <c r="L69" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" s="3"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
         <v>138</v>
       </c>
@@ -2424,16 +2325,13 @@
       <c r="K72">
         <v>0</v>
       </c>
-      <c r="L72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -2467,11 +2365,8 @@
       <c r="K75">
         <v>1000</v>
       </c>
-      <c r="L75">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -2505,11 +2400,8 @@
       <c r="K76">
         <v>5</v>
       </c>
-      <c r="L76">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>23</v>
       </c>
@@ -2543,11 +2435,8 @@
       <c r="K77">
         <v>5</v>
       </c>
-      <c r="L77">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>23</v>
       </c>
@@ -2581,11 +2470,8 @@
       <c r="K78">
         <v>15</v>
       </c>
-      <c r="L78">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>52</v>
       </c>
@@ -2593,10 +2479,11 @@
         <v>51</v>
       </c>
       <c r="C79">
+        <f t="shared" ref="C79:K79" si="0">-5/12*PI()</f>
         <v>-1.3089969389957472</v>
       </c>
       <c r="D79">
-        <f t="shared" ref="D79:L79" si="0">-5/12*PI()</f>
+        <f t="shared" si="0"/>
         <v>-1.3089969389957472</v>
       </c>
       <c r="E79">
@@ -2627,12 +2514,8 @@
         <f t="shared" si="0"/>
         <v>-1.3089969389957472</v>
       </c>
-      <c r="L79">
-        <f t="shared" si="0"/>
-        <v>-1.3089969389957472</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>52</v>
       </c>
@@ -2640,10 +2523,11 @@
         <v>53</v>
       </c>
       <c r="C80">
+        <f t="shared" ref="C80:K80" si="1">5/12*PI()</f>
         <v>1.3089969389957472</v>
       </c>
       <c r="D80">
-        <f t="shared" ref="D80:L80" si="1">5/12*PI()</f>
+        <f t="shared" si="1"/>
         <v>1.3089969389957472</v>
       </c>
       <c r="E80">
@@ -2674,12 +2558,8 @@
         <f t="shared" si="1"/>
         <v>1.3089969389957472</v>
       </c>
-      <c r="L80">
-        <f t="shared" si="1"/>
-        <v>1.3089969389957472</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>55</v>
       </c>
@@ -2687,10 +2567,11 @@
         <v>54</v>
       </c>
       <c r="C81">
+        <f t="shared" ref="C81:K81" si="2">11/6*PI()</f>
         <v>5.7595865315812871</v>
       </c>
       <c r="D81">
-        <f t="shared" ref="D81:L81" si="2">11/6*PI()</f>
+        <f t="shared" si="2"/>
         <v>5.7595865315812871</v>
       </c>
       <c r="E81">
@@ -2721,12 +2602,8 @@
         <f t="shared" si="2"/>
         <v>5.7595865315812871</v>
       </c>
-      <c r="L81">
-        <f t="shared" si="2"/>
-        <v>5.7595865315812871</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B82" t="s">
         <v>56</v>
       </c>
@@ -2757,11 +2634,8 @@
       <c r="K82">
         <v>-1.8429999999999998E-2</v>
       </c>
-      <c r="L82">
-        <v>-1.8429999999999998E-2</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B83" t="s">
         <v>57</v>
       </c>
@@ -2792,19 +2666,17 @@
       <c r="K83">
         <v>0.37819999999999998</v>
       </c>
-      <c r="L83">
-        <v>0.37819999999999998</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B84" t="s">
         <v>58</v>
       </c>
       <c r="C84">
+        <f t="shared" ref="C84:K84" si="3">-2.3782</f>
         <v>-2.3782000000000001</v>
       </c>
       <c r="D84">
-        <f t="shared" ref="D84:L84" si="3">-2.3782</f>
+        <f t="shared" si="3"/>
         <v>-2.3782000000000001</v>
       </c>
       <c r="E84">
@@ -2835,12 +2707,8 @@
         <f t="shared" si="3"/>
         <v>-2.3782000000000001</v>
       </c>
-      <c r="L84">
-        <f t="shared" si="3"/>
-        <v>-2.3782000000000001</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -2874,16 +2742,13 @@
       <c r="K85">
         <v>4</v>
       </c>
-      <c r="L85">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B88" t="s">
         <v>60</v>
       </c>
@@ -2914,11 +2779,8 @@
       <c r="K88" t="s">
         <v>61</v>
       </c>
-      <c r="L88" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B89" t="s">
         <v>62</v>
       </c>
@@ -2949,11 +2811,8 @@
       <c r="K89" t="s">
         <v>63</v>
       </c>
-      <c r="L89" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B90" t="s">
         <v>64</v>
       </c>
@@ -2984,11 +2843,8 @@
       <c r="K90" t="s">
         <v>65</v>
       </c>
-      <c r="L90" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>68</v>
       </c>
@@ -3022,15 +2878,12 @@
       <c r="K91" t="s">
         <v>67</v>
       </c>
-      <c r="L91" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B92" t="s">
         <v>69</v>
       </c>
-      <c r="C92" t="b">
+      <c r="C92" s="4" t="b">
         <v>1</v>
       </c>
       <c r="D92" s="4" t="b">
@@ -3057,11 +2910,8 @@
       <c r="K92" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="L92" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B93" t="s">
         <v>70</v>
       </c>
@@ -3092,11 +2942,8 @@
       <c r="K93" t="b">
         <v>1</v>
       </c>
-      <c r="L93" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B94" t="s">
         <v>71</v>
       </c>
@@ -3127,11 +2974,8 @@
       <c r="K94" t="b">
         <v>0</v>
       </c>
-      <c r="L94" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B95" t="s">
         <v>72</v>
       </c>
@@ -3162,11 +3006,8 @@
       <c r="K95" t="b">
         <v>1</v>
       </c>
-      <c r="L95" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B96" t="s">
         <v>73</v>
       </c>
@@ -3197,11 +3038,8 @@
       <c r="K96" t="b">
         <v>1</v>
       </c>
-      <c r="L96" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B97" t="s">
         <v>74</v>
       </c>
@@ -3232,13 +3070,10 @@
       <c r="K97" t="b">
         <v>0</v>
       </c>
-      <c r="L97" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B98" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C98" t="b">
         <v>0</v>
@@ -3267,13 +3102,10 @@
       <c r="K98" t="b">
         <v>0</v>
       </c>
-      <c r="L98" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B99" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C99" t="b">
         <v>0</v>
@@ -3302,16 +3134,13 @@
       <c r="K99" t="b">
         <v>0</v>
       </c>
-      <c r="L99" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B102" t="s">
         <v>76</v>
       </c>
@@ -3342,11 +3171,8 @@
       <c r="K102" t="s">
         <v>77</v>
       </c>
-      <c r="L102" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B103" t="s">
         <v>78</v>
       </c>
@@ -3377,11 +3203,8 @@
       <c r="K103">
         <v>50</v>
       </c>
-      <c r="L103">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>89</v>
       </c>
@@ -3415,11 +3238,8 @@
       <c r="K104">
         <v>50</v>
       </c>
-      <c r="L104">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>23</v>
       </c>
@@ -3453,11 +3273,8 @@
       <c r="K105">
         <v>0</v>
       </c>
-      <c r="L105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>23</v>
       </c>
@@ -3491,11 +3308,8 @@
       <c r="K106">
         <v>0</v>
       </c>
-      <c r="L106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>16</v>
       </c>
@@ -3529,11 +3343,8 @@
       <c r="K107">
         <v>500</v>
       </c>
-      <c r="L107">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>16</v>
       </c>
@@ -3567,11 +3378,8 @@
       <c r="K108">
         <v>800</v>
       </c>
-      <c r="L108">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>93</v>
       </c>
@@ -3605,11 +3413,8 @@
       <c r="K109">
         <v>8</v>
       </c>
-      <c r="L109">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>93</v>
       </c>
@@ -3643,11 +3448,8 @@
       <c r="K110">
         <v>8</v>
       </c>
-      <c r="L110">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>92</v>
       </c>
@@ -3681,11 +3483,8 @@
       <c r="K111">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="L111">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>90</v>
       </c>
@@ -3719,11 +3518,8 @@
       <c r="K112">
         <v>2000</v>
       </c>
-      <c r="L112">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>91</v>
       </c>
@@ -3757,16 +3553,13 @@
       <c r="K113">
         <v>4000</v>
       </c>
-      <c r="L113">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B116" t="s">
         <v>95</v>
       </c>
@@ -3797,11 +3590,8 @@
       <c r="K116" t="s">
         <v>97</v>
       </c>
-      <c r="L116" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.45">
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B117" t="s">
         <v>96</v>
       </c>
@@ -3830,9 +3620,6 @@
         <v>98</v>
       </c>
       <c r="K117" t="s">
-        <v>98</v>
-      </c>
-      <c r="L117" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MasterScriptAdam uses read/write cell, parfor calls helper function to save struct and eval
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hombo\Documents\Github Repositories\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\Code of Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762BB8DC-B40B-48B6-BAF0-C3447A44778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6C8468-4D6B-4495-A2F8-2296F96FC094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -833,7 +833,7 @@
   <dimension ref="A1:K117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D5" sqref="D5:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -852,27 +852,6 @@
       <c r="C1">
         <v>1</v>
       </c>
-      <c r="D1">
-        <v>2</v>
-      </c>
-      <c r="E1">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>4</v>
-      </c>
-      <c r="G1">
-        <v>5</v>
-      </c>
-      <c r="H1">
-        <v>6</v>
-      </c>
-      <c r="I1">
-        <v>7</v>
-      </c>
-      <c r="J1">
-        <v>8</v>
-      </c>
       <c r="K1">
         <v>9</v>
       </c>
@@ -925,31 +904,31 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="D5">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="E5">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="F5">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="G5">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="H5">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="I5">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="J5">
-        <v>1800</v>
+        <v>150</v>
       </c>
       <c r="K5">
-        <v>1800</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
@@ -1217,6 +1196,11 @@
         <v>1</v>
       </c>
       <c r="K13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="D14">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deleted lots of old files
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim Draft 1/Code of Laws/AdamsLaw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hombo\Documents\Github Repositories\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim Draft 1\Code of Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6C8468-4D6B-4495-A2F8-2296F96FC094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D205125B-4955-44ED-8D49-CC9DF19AB0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -327,9 +327,6 @@
     <t>funcName_findNeighborhood</t>
   </si>
   <si>
-    <t>agentControl_Adam</t>
-  </si>
-  <si>
     <t>findNeighborhood_fixedRadius</t>
   </si>
   <si>
@@ -499,6 +496,9 @@
   </si>
   <si>
     <t>[1,4]</t>
+  </si>
+  <si>
+    <t>agentControl_ManyFactors</t>
   </si>
 </sst>
 </file>
@@ -832,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:K5"/>
+    <sheetView tabSelected="1" topLeftCell="B100" workbookViewId="0">
+      <selection activeCell="H118" sqref="H118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -847,7 +847,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -904,7 +904,7 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>150</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -928,7 +928,7 @@
         <v>150</v>
       </c>
       <c r="K5">
-        <v>150</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
@@ -1073,7 +1073,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" t="b">
         <v>1</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12" t="b">
         <v>1</v>
@@ -1169,7 +1169,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1362,31 +1362,31 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
@@ -1461,207 +1461,207 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" t="s">
         <v>133</v>
       </c>
-      <c r="C32" t="s">
-        <v>134</v>
-      </c>
       <c r="D32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" t="s">
         <v>115</v>
       </c>
-      <c r="B35" t="s">
-        <v>116</v>
-      </c>
       <c r="C35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K35" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" t="s">
         <v>118</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>119</v>
       </c>
-      <c r="C36" t="s">
-        <v>120</v>
-      </c>
       <c r="D36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.45">
@@ -1708,80 +1708,80 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C45" t="s">
+        <v>149</v>
+      </c>
+      <c r="D45" t="s">
         <v>150</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>151</v>
       </c>
-      <c r="E45" t="s">
-        <v>152</v>
-      </c>
       <c r="F45" t="s">
+        <v>149</v>
+      </c>
+      <c r="G45" t="s">
         <v>150</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>151</v>
       </c>
-      <c r="H45" t="s">
-        <v>152</v>
-      </c>
       <c r="I45" t="s">
+        <v>149</v>
+      </c>
+      <c r="J45" t="s">
         <v>150</v>
       </c>
-      <c r="J45" t="s">
+      <c r="K45" t="s">
         <v>151</v>
-      </c>
-      <c r="K45" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" t="s">
         <v>123</v>
       </c>
-      <c r="B46" t="s">
-        <v>124</v>
-      </c>
       <c r="C46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K46" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B47" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1850,80 +1850,80 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C53">
         <v>2000</v>
@@ -1992,82 +1992,82 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B58" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C61">
         <v>6</v>
@@ -2150,37 +2150,37 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" t="s">
         <v>131</v>
       </c>
-      <c r="B65" t="s">
-        <v>132</v>
-      </c>
       <c r="C65" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.45">
@@ -2272,15 +2272,15 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B72" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -2697,7 +2697,7 @@
         <v>16</v>
       </c>
       <c r="B85" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C85">
         <v>4</v>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B98" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C98" t="b">
         <v>0</v>
@@ -3089,7 +3089,7 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B99" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C99" t="b">
         <v>0</v>
@@ -3548,31 +3548,31 @@
         <v>95</v>
       </c>
       <c r="C116" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="D116" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="E116" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="F116" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="G116" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="H116" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="I116" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="J116" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="K116" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.45">
@@ -3580,31 +3580,31 @@
         <v>96</v>
       </c>
       <c r="C117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>